<commit_message>
AFDP-9108 Fix Consultation Module Admin Issues
- Add consultation as object type in admin module
- Add consultation as possible parent of costsheets and timesheets
- Insert default type on Consultation save
- Fix change consultation status workflow and modal not showing approvers/reviewers
</commit_message>
<xml_diff>
--- a/acm/rules/drools-consultation-rules.xlsx
+++ b/acm/rules/drools-consultation-rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksandar.acevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7A80C3-E73C-481E-BFEC-2DBBC9A821E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DBAB76-7314-49B1-8BB4-5E232345B8B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10350" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>RuleSet</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>Save Consultation File Rules</t>
+  </si>
+  <si>
+    <t>Set Consultation Type</t>
+  </si>
+  <si>
+    <t>setConsultationType, 'Consultation'</t>
+  </si>
+  <si>
+    <t>consultationType == null || consultationType.equals("")</t>
   </si>
 </sst>
 </file>
@@ -849,23 +858,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D33"/>
+  <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.42578125"/>
-    <col min="2" max="2" width="24.28515625"/>
-    <col min="3" max="3" width="50.140625"/>
-    <col min="4" max="4" width="100.42578125"/>
-    <col min="5" max="5" width="27.7109375"/>
-    <col min="6" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="19.3984375"/>
+    <col min="2" max="2" width="24.265625"/>
+    <col min="3" max="3" width="50.1328125"/>
+    <col min="4" max="4" width="100.3984375"/>
+    <col min="5" max="5" width="27.73046875"/>
+    <col min="6" max="1025" width="8.73046875"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -875,7 +884,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -885,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -895,7 +904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -905,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -915,7 +924,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -925,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -935,7 +944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -945,7 +954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -955,7 +964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -965,7 +974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -975,7 +984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -985,7 +994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="330" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="313.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -995,7 +1004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -1005,7 +1014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -1013,7 +1022,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -1023,7 +1032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -1031,7 +1040,7 @@
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -1041,7 +1050,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -1055,7 +1064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>37</v>
@@ -1067,7 +1076,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>22</v>
@@ -1079,7 +1088,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>39</v>
@@ -1091,71 +1100,83 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="1"/>
+      <c r="B27" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D27" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="1"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1169,9 +1190,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375"/>
+    <col min="1" max="1025" width="8.73046875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1185,9 +1206,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375"/>
+    <col min="1" max="1025" width="8.73046875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>